<commit_message>
hnd name pattern added and conditions changes
</commit_message>
<xml_diff>
--- a/Data/fullnamelist.xlsx
+++ b/Data/fullnamelist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python Code\Best-on-Python\short_naming\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python Code\Short-Name-Generator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03FA8485-CDFE-46E1-8EDF-726BFF0A4D34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69AA1D44-1015-4C9A-9896-42E567C3E40C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="887">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1457" uniqueCount="1288">
   <si>
     <t xml:space="preserve">Hazra Pharmacy                                              </t>
   </si>
@@ -2686,6 +2686,1209 @@
   </si>
   <si>
     <t>fullname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Classic Provita Agro Ltd.                                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shaba &amp; Diba Poultry                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Satata Poultry                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shahjalal Feed House                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Akbar Poultry                                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ashik Enterprise                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TONGWEI FEED MILL (BANGLADESH) CO. LTD.                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adnan Agro Ltd.                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chhuya Agro Products Ltd.                                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provita Feed Ltd.                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provita Breeders Ltd                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nurani Poultry &amp; Fishery Ready Feed Ltd.                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sunrise Poultry &amp; Hatchery Ltd.                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tasnim Pharmacy                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Srizonshil Agro Farm                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mama Vagina Enterprise                                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FatimaPharmacy                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">B K Poultry                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bismillah Veterinary                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asif Towa Pharmacy                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moon Traders                                                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MS Era Poultry                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nusrat Vet Medicine                                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sotota Veterinary Medicine Corner                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Veterinary Point                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arafat Veterinary                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joynal Traders                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R. R. P Farms                                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protein House Ltd.                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nice Farms Ltd.                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hazi Poultry Feed Mill                                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">North's Egg Ltd.                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diamond Chicks Ltd.                                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asa Poultry &amp; Hatchery                                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ekramul Haque Agro Industries Ltd.                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goalondo Poultry Feed                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maa Medicine corner                                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Islam medical hall                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biswas Feed Centre                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aziron Poultry Feed &amp; Medicine                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samiya Poultry Feed Center                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kazi Enterprise                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raton Medical Hall                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nupur Pharmacy                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tota Enterprise                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ashuk Traders                                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sohel Pharmacy                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sondha Pharmacy                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shabul Traders                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Musfika Traders                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bangladesh Medical Veterinary                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Akhon Poultry Feed                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mitali Drug House                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tanvir Traders                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Artho Agro Traders                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Papia Medicine Corner                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Janoni Pharmacy                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jahid Pharmacy                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adnan Enterprise                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shaif Agro House                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rokeya Fish Feed                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raj Medical Hall                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joint Poultry                                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fatima Enterprise                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mama Vagna Traders                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ruhan Traders                                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Puspo Medical Hall                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moumita Enterprise                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mayer Doya Enterprise                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sikder Medicine Centre                                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mainuddin Medical Hall                                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mirza Medical Hall                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biplob Kitnashok Biponi                                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bismillah Enterprise                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simanto Poultry                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ma Medicine Store                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anamul Enterprise                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yeaser Poultry Farm &amp; Fish Feed                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Narendran Medical Hall                                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sheikh Traders                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rony Poultry Feed                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haldar Feeds                                                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nihan Poultry &amp; Feed                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mollah Enterprise                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Janoni Poultry                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bondhu Poultry Feed                                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Akib Medical Hall                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jashim Medical Hall                                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Veterinary care center &amp; pharmacy                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">P Pharmacy                                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shahin Veterinary                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pramanik Pharmacy                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Himel Traders                                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Akota Poultry And Feed                                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Al Modina Enterprise                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bismillah Enterprise 3                                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faisal Poultry Complex                                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taheria Traders                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vet Doctor Point                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xion Medicine Corner                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nurunnahar Veterinary                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tamim Agro Industries Ltd.                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Polloby Pharmacy                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bismillah Medical Hall 3                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raza Pharmacy                                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maa Vetenirary Pharmacy                                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peoples Poultry &amp; Hatchery Ltd.                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Polish Fish Feed                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asad Medical Hall                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bismillah Treders                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuhin Enterprise                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ma Fatema Enterprise                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bhai bhai Traders                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Nuha Store                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mitali Traders                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shaba Medical Hall                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sham Fisheries                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kamrul  Hasan Medical  Hall                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mesars Hamim  Treders                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mayer Doa Enterprise                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hasi Medical Store                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diamond Eggs Ltd.                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zihad Poultry &amp; Dairy Medicine Corner                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Science Met                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bhai Bhai Enterprise                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M S Masud Medical Store                                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chandon Pharmacy                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allahar Dan Pharmacy                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bego Pharmacy                                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moiniya  Pharmacy                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shaikh Brothers                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Partha Pharmacy                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mollick Aushadh Ghar                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Afia Drug House                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anowarul Veterinary Pharmacy                                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mohona Pharmacy                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faruk Veterinary Hall                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mim Veterinary &amp; Fisharise                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Al Modina Hatcher                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jubair Enterprise &amp; Fish Feed                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taiyaba Pharmacy                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miran Veterinary Drug House                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barik Enterprise                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fatema Enterprise                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Labonno Enterprise                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ayshi Medical                                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ma Moni Medical                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abu Bokkor Siddique Enterprise                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rosulpur Pharmacy                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mubasir Pharmacy                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> M S Narju Poultry &amp; Fish Feed                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ma Babar Doa Veterinary Osadholay                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nasir Traders                                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rimi Enterprise                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shanaz Pharmacy                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shahab Pharmacy                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M S Kashem Enterprise                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sathi Traders                                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biplob Agro &amp; Fish                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antor Poultry &amp; Fisharish                                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joy Bijoy Pharmacy                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Japfa Comfeed Bangladesh Pte Ltd.                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quality Breeders Ltd.                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provita Hatcheries Ltd.                                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Akota Feed &amp; Medicine                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">J R Poultry                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ahmed Enterprise                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nazrul Dairy Farm &amp; Medicin Corner                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mokka Pharmacy                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eyda Medical Hall                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adia Enterprise                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rabeya Enterprise                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simanto Dairy Farm                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGATA Feed Mills Ltd.                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pulin Pharmacy                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sakib Enterprise                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Humayan Trders                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Takwa Agro Traders                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bismillah Traders                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ausim Medicine Corner                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anika Veterinary                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Islamia Medical Hall                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maa Babar Doya Medicine House                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Al Amin Store                                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alif Poltry &amp; Dairy Medicine                                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tanvir Medical Hall                                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bhai Bhai Poultry Feed                                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M S Habib Traders                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sadiya Fisheries                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">J.R.Prani sastho Pharmacy                                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Habib Motso Khamar                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anowara Pharmacy                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diya Pharmacy                                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muhin Pharmacy                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kobir Enterprise                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Polly Aushad Ghar                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maidul Traders                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saifa Agro                                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Madina Traders                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alam Maya Poultry Feed                                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bhai Bhai Poultry                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mayer Doya Traders                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monir Veterinary                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jenifa Pharmacy &amp; Poultry                                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barsha Poultry Feed &amp; Medicine                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Siddikur Enterprise                                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Talukder Medical Hall                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mugdho Enterprise                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saad Medical Hall                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ema Pharmacy                                                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Talukder Veterinary &amp;  Pharmacy                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imon Pharmacy                                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sifat poultry                                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nazma Medical Hall                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Niamotullah Medical Hall                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Al Riyad Poultry Feed                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moni Store                                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grameen Medical Hall                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abdur Rahman Homio &amp; Vet                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">New M S Pharmacy                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Turfa Pharmacy                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sun Agro industries Ltd.                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saddam Medical Hall                                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monira Vet &amp; Animals Feed                                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datta Medical Store                                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ma Poultry                                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bio Agro BD  Rangpur                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drug Palace                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reaz Feed Seba                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tamim Poultry Feed                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ripa Enterprise                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">S S Poultry                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abdullah Poultry Feed                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nafi Model Medicine Shop                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Humaysha Fish Feed                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M S khushi Model Medicine Shop                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maa  Babar Doya  Medicine Corner                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arafat Pharmacy                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bikash Pharmacy                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Khondokar Pharmacy                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nayem Medical Hall                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aman Poultry &amp; Hatchery Ltd.                                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nourish Poultry &amp; Hatchery                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nahar Agro Complex                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aftab Bahumukhi Farm Limited                                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shadesh Farms Ltd.                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Hope Feed Mill BD. Ltd.                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Akhanda Poultry Feed                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">German Poultry Farm                                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abrar Traders                                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Babul Poultry Feed                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arafat Trades                                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aman Breeders Ltd                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Siam Pharmacy                                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mukti Veterinary Medicine Corner                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prem Business Line                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ma Poultry and Dairy                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">F K Traders                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Safara Agro Industries                                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AG Agro Industries Limited                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quality Feeds Limited                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selim Medical Hall                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mayer Doya Medicine House                                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Runa Pharmacy                                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mosarof poultry &amp; fish feed center                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joya Traders                                                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dey Pharmacy                                                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.R Poultry &amp; Fish Feed                                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Polly Praniseba Medical Hall                                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abdullah Al Ruman Store                                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uddin store                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reza Pharmacy                                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chacha Vatiza Agro                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sayed Phamacy                                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jihan Abdullah Trader s                                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juthi Prani Pusti                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suvo Traders                                                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hajrot Medical Hall                                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shoyab Traders                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unity Poultry Complex                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nur Medicine Center                                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shaha Poultry Feed And Chick                                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jubayer Poultry Feed &amp; Madicine                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mukter Pharmacy                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mama Vagina Poultry Feed                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sumon Traders                                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shaikh Poultry                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sadika Pharmacy                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ruma Pharmacy                                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AB Medicine                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zinnah Pharmacy                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mehedi Hasan Pharmacy                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mayer Doua Pharmacy                                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bhai Bhai  Pharmacy                                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rakib Pharmacy                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Masud Rana Medical                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M S Ridoy Poultry Feed                                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">karim Pharmacy                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Noman Veterinary                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mayer Doya Poultry Feed                                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sumon Poultry &amp; Feed                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zinak Poultry &amp; Feed                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A N Enterprise                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Othithi Poultry Feed &amp; Medicine                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Murad Enterprise                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Farij Medical Hall                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shafiq Pharmacy                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amjad veterinary                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mollah Medical Hall                                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kazi Foods Limited                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Habiba Traders                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bondhan Pharmacy                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asian Agro Farm                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kamona Medical Store                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tawhid Pharmacy                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mithun Enterprise                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ma Poultry &amp; Feed                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">K N A Enterprise                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Islam Enterprise                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AG Broilers Ltd.                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abir Poultry Ltd.                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C.P. Bangladesh Co., Ltd                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AG GP Ltd.                                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rashid Krishi Khamar                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sunny Feeds Limited                                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Index Poultry Pvt. Ltd.                                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maa Duggar House                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maa babar Ashirbad                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M S Haque Pharmacy                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moon Veterinary                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ayan Poultry Feed &amp; Medicine Center                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bangla Feed Mill                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Natural Motsho Khamar                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shafa Pharmacy                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M S Tabassum Model Medicine Shop                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zaman Fish                                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jononi Fish Feed &amp; Poultry                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forazi Enterprise                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salam Enterpise                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mathbor Pharmacy                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prottasa Pharmacy                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toufika Traders                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maa Veterinary Store                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lucky Pharmacy                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">S K Traders                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mominul Enterprise                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abdur Rahim Traders                                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lorin Pharmacy                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amin Pharmacy                                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juba Fish &amp; Medicine Store                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tabassum Traders                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zim Poultry                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maa Poultry Farm                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mocca Modina Agro                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nadim Medical Store                                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MS Bhai Bhai Traders                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saif Medical Hall                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bhuiyan Checks &amp; feed                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Korim Traders                                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sadiq Poultry                                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maa Baba Veterinary                                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anowara Poultry &amp; Feed s                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maisha Veterinary Store                                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neshit Traders                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rupayen Medical hall                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Talukder Veterinary &amp; Krittim Projonon Kendro               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mukta Traders                                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maa Babar Doya Veterinary &amp; Poultry                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hawlader Traders 3                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saber Medical Hall                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">S.P.L Pharma                                                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amanot Poultry                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Al Amin Veterinary                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mizan Pharmacy                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shohidul Hatchery                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Khondokar Feed &amp; Fish                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Janani Trade Center                                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sani Medical                                                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Al Nur Pharmacy                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TM Agro Feed                                                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Somiron Laibrary                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ali Medical Hall                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dr. Emran Hossain Pharmacy                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Advanced Golden Eggs &amp; Chicks Ltd.                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arinjoy Krishi Vandar                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anwar Fish Feed                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ma Ousadh Ghar                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kalam Pharmacy                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alom Traders                                                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sunny Breeders Ltd.                                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Farhana Medical Hall                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nusrat Traders                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smriti Poultry &amp; Fish Feed                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hussain Poultry Feed                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arif Veterinary                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shuvo Enterprise                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gobadi Poshu Chikishaloy                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baba Mayer Doa                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ma Babar Doa Veterinary                                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nasra Agro Ltd                                              </t>
+  </si>
+  <si>
+    <t>HND Data</t>
   </si>
 </sst>
 </file>
@@ -2721,7 +3924,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -3003,9 +4207,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A1006"/>
+  <dimension ref="A1:A1457"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A994" workbookViewId="0">
+      <selection activeCell="A1008" sqref="A1008"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -8042,6 +9248,2261 @@
         <v>885</v>
       </c>
     </row>
+    <row r="1007" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1007" t="s">
+        <v>1287</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1008" s="1" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1009" s="1" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1010" s="1" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1011" s="1" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1012" s="1" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1013" s="1" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1014" s="1" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1015" s="1" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1016" s="1" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1017" s="1" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1018" s="1" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1019" s="1" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1020" s="1" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1021" s="1" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1022" s="1" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1023" s="1" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="1024" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1024" s="1" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="1025" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1025" s="1" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="1026" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1026" s="1" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1027" s="1" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1028" s="1" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="1029" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1029" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="1030" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1030" s="1" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="1031" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1031" s="1" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1032" s="1" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="1033" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1033" s="1" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="1034" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1034" s="1" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="1035" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1035" s="1" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="1036" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1036" s="1" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="1037" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1037" s="1" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="1038" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1038" s="1" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="1039" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1039" s="1" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="1040" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1040" s="1" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="1041" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1041" s="1" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="1042" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1042" s="1" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="1043" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1043" s="1" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="1044" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1044" s="1" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="1045" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1045" s="1" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="1046" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1046" s="1" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="1047" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1047" s="1" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="1048" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1048" s="1" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="1049" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1049" s="1" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1050" s="1" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1051" s="1" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="1052" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1052" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="1053" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1053" s="1" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="1054" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1054" s="1" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="1055" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1055" s="1" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1056" s="1" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1057" s="1" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="1058" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1058" s="1" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="1059" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1059" s="1" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1060" s="1" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1061" s="1" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1062" s="1" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="1063" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1063" s="1" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1064" s="1" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="1065" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1065" s="1" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="1066" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1066" s="1" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="1067" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1067" s="1" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="1068" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1068" s="1" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="1069" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1069" s="1" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1070" s="1" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="1071" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1071" s="1" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="1072" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1072" s="1" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="1073" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1073" s="1" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="1074" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1074" s="1" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="1075" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1075" s="1" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="1076" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1076" s="1" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="1077" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1077" s="1" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="1078" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1078" s="1" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="1079" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1079" s="1" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="1080" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1080" s="1" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="1081" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1081" s="1" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="1082" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1082" s="1" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="1083" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1083" s="1" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="1084" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1084" s="1" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="1085" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1085" s="1" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="1086" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1086" s="1" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="1087" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1087" s="1" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="1088" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1088" s="1" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="1089" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1089" s="1" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="1090" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1090" s="1" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="1091" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1091" s="1" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="1092" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1092" s="1" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="1093" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1093" s="1" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="1094" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1094" s="1" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="1095" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1095" s="1" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="1096" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1096" s="1" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="1097" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1097" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1098" s="1" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1099" s="1" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="1100" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1100" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="1101" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1101" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="1102" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1102" s="1" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1103" s="1" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1104" s="1" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1105" s="1" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1106" s="1" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="1107" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1107" s="1" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1108" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1109" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1109" s="1" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="1110" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1110" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="1111" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1111" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="1112" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1112" s="1" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="1113" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1113" s="1" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="1114" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1114" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="1115" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1115" s="1" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="1116" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1116" s="1" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="1117" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1117" s="1" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="1118" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1118" s="1" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="1119" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1119" s="1" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="1120" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1120" s="1" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="1121" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1121" s="1" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="1122" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1122" s="1" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="1123" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1123" s="1" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="1124" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1124" s="1" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="1125" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1125" s="1" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="1126" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1126" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="1127" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1127" s="1" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="1128" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1128" s="1" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="1129" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1129" s="1" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="1130" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1130" s="1" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="1131" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1131" s="1" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="1132" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1132" s="1" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="1133" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1133" s="1" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="1134" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1134" s="1" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="1135" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1135" s="1" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="1136" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1136" s="1" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="1137" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1137" s="1" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="1138" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1138" s="1" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="1139" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1139" s="1" t="s">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="1140" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1140" s="1" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="1141" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1141" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="1142" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1142" s="1" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="1143" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1143" s="1" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1144" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1144" s="1" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="1145" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1145" s="1" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="1146" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1146" s="1" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="1147" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1147" s="1" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="1148" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1148" s="1" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="1149" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1149" s="1" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="1150" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1150" s="1" t="s">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="1151" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1151" s="1" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="1152" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1152" s="1" t="s">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="1153" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1153" s="1" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="1154" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1154" s="1" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="1155" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1155" s="1" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="1156" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1156" s="1" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="1157" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1157" s="1" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="1158" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1158" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1159" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1159" s="1" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="1160" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1160" s="1" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="1161" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1161" s="1" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="1162" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1162" s="1" t="s">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="1163" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1163" s="1" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="1164" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1164" s="1" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="1165" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1165" s="1" t="s">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="1166" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1166" s="1" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="1167" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1167" s="1" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="1168" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1168" s="1" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="1169" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1169" s="1" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="1170" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1170" s="1" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="1171" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1171" s="1" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="1172" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1172" s="1" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="1173" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1173" s="1" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="1174" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1174" s="1" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="1175" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1175" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="1176" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1176" s="1" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="1177" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1177" s="1" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="1178" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1178" s="1" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="1179" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1179" s="1" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="1180" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1180" s="1" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="1181" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1181" s="1" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="1182" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1182" s="1" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="1183" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1183" s="1" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="1184" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1184" s="1" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="1185" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1185" s="1" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="1186" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1186" s="1" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="1187" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1187" s="1" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="1188" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1188" s="1" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="1189" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1189" s="1" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="1190" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1190" s="1" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="1191" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1191" s="1" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="1192" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1192" s="1" t="s">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="1193" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1193" s="1" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="1194" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1194" s="1" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="1195" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1195" s="1" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="1196" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1196" s="1" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="1197" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1197" s="1" t="s">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="1198" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1198" s="1" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="1199" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1199" s="1" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="1200" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1200" s="1" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="1201" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1201" s="1" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="1202" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1202" s="1" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="1203" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1203" s="1" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="1204" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1204" s="1" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="1205" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1205" s="1" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="1206" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1206" s="1" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="1207" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1207" s="1" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="1208" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1208" s="1" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="1209" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1209" s="1" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="1210" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1210" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="1211" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1211" s="1" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="1212" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1212" s="1" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="1213" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1213" s="1" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="1214" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1214" s="1" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="1215" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1215" s="1" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="1216" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1216" s="1" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="1217" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1217" s="1" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="1218" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1218" s="1" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="1219" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1219" s="1" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="1220" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1220" s="1" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="1221" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1221" s="1" t="s">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="1222" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1222" s="1" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="1223" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1223" s="1" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="1224" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1224" s="1" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="1225" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1225" s="1" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="1226" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1226" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="1227" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1227" s="1" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="1228" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1228" s="1" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="1229" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1229" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="1230" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1230" s="1" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="1231" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1231" s="1" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="1232" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1232" s="1" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="1233" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1233" s="1" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="1234" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1234" s="1" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="1235" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1235" s="1" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="1236" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1236" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="1237" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1237" s="1" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="1238" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1238" s="1" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="1239" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1239" s="1" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="1240" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1240" s="1" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="1241" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1241" s="1" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="1242" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1242" s="1" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="1243" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1243" s="1" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="1244" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1244" s="1" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="1245" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1245" s="1" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="1246" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1246" s="1" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="1247" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1247" s="1" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="1248" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1248" s="1" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="1249" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1249" s="1" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="1250" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1250" s="1" t="s">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="1251" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1251" s="1" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="1252" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1252" s="1" t="s">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="1253" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1253" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1254" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1254" s="1" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="1255" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1255" s="1" t="s">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="1256" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1256" s="1" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="1257" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1257" s="1" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="1258" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1258" s="1" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="1259" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1259" s="1" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="1260" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1260" s="1" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="1261" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1261" s="1" t="s">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="1262" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1262" s="1" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="1263" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1263" s="1" t="s">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="1264" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1264" s="1" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="1265" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1265" s="1" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="1266" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1266" s="1" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="1267" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1267" s="1" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="1268" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1268" s="1" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="1269" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1269" s="1" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="1270" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1270" s="1" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="1271" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1271" s="1" t="s">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="1272" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1272" s="1" t="s">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="1273" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1273" s="1" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="1274" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1274" s="1" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="1275" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1275" s="1" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1276" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1276" s="1" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="1277" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1277" s="1" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="1278" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1278" s="1" t="s">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="1279" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1279" s="1" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="1280" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1280" s="1" t="s">
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="1281" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1281" s="1" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="1282" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1282" s="1" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="1283" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1283" s="1" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="1284" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1284" s="1" t="s">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="1285" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1285" s="1" t="s">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="1286" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1286" s="1" t="s">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="1287" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1287" s="1" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="1288" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1288" s="1" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="1289" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1289" s="1" t="s">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="1290" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1290" s="1" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="1291" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1291" s="1" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="1292" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1292" s="1" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="1293" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1293" s="1" t="s">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="1294" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1294" s="1" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="1295" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1295" s="1" t="s">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="1296" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1296" s="1" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="1297" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1297" s="1" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="1298" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1298" s="1" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="1299" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1299" s="1" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="1300" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1300" s="1" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="1301" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1301" s="1" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="1302" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1302" s="1" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="1303" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1303" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="1304" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1304" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="1305" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1305" s="1" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="1306" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1306" s="1" t="s">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="1307" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1307" s="1" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="1308" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1308" s="1" t="s">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="1309" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1309" s="1" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="1310" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1310" s="1" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="1311" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1311" s="1" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="1312" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1312" s="1" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="1313" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1313" s="1" t="s">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="1314" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1314" s="1" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="1315" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1315" s="1" t="s">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="1316" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1316" s="1" t="s">
+        <v>1163</v>
+      </c>
+    </row>
+    <row r="1317" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1317" s="1" t="s">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="1318" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1318" s="1" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="1319" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1319" s="1" t="s">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="1320" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1320" s="1" t="s">
+        <v>1166</v>
+      </c>
+    </row>
+    <row r="1321" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1321" s="1" t="s">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="1322" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1322" s="1" t="s">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="1323" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1323" s="1" t="s">
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="1324" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1324" s="1" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="1325" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1325" s="1" t="s">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="1326" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1326" s="1" t="s">
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="1327" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1327" s="1" t="s">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="1328" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1328" s="1" t="s">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="1329" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1329" s="1" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="1330" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1330" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="1331" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1331" s="1" t="s">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="1332" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1332" s="1" t="s">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="1333" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1333" s="1" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="1334" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1334" s="1" t="s">
+        <v>1178</v>
+      </c>
+    </row>
+    <row r="1335" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1335" s="1" t="s">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="1336" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1336" s="1" t="s">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="1337" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1337" s="1" t="s">
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="1338" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1338" s="1" t="s">
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="1339" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1339" s="1" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="1340" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1340" s="1" t="s">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="1341" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1341" s="1" t="s">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="1342" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1342" s="1" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="1343" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1343" s="1" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="1344" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1344" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1345" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1345" s="1" t="s">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="1346" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1346" s="1" t="s">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="1347" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1347" s="1" t="s">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="1348" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1348" s="1" t="s">
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="1349" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1349" s="1" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="1350" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1350" s="1" t="s">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="1351" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1351" s="1" t="s">
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="1352" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1352" s="1" t="s">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="1353" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1353" s="1" t="s">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="1354" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1354" s="1" t="s">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="1355" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1355" s="1" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="1356" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1356" s="1" t="s">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="1357" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1357" s="1" t="s">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="1358" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1358" s="1" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="1359" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1359" s="1" t="s">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="1360" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1360" s="1" t="s">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="1361" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1361" s="1" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="1362" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1362" s="1" t="s">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="1363" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1363" s="1" t="s">
+        <v>1204</v>
+      </c>
+    </row>
+    <row r="1364" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1364" s="1" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="1365" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1365" s="1" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="1366" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1366" s="1" t="s">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="1367" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1367" s="1" t="s">
+        <v>1207</v>
+      </c>
+    </row>
+    <row r="1368" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1368" s="1" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="1369" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1369" s="1" t="s">
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="1370" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1370" s="1" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="1371" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1371" s="1" t="s">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="1372" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1372" s="1" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="1373" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1373" s="1" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="1374" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1374" s="1" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="1375" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1375" s="1" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="1376" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1376" s="1" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="1377" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1377" s="1" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="1378" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1378" s="1" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="1379" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1379" s="1" t="s">
+        <v>1217</v>
+      </c>
+    </row>
+    <row r="1380" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1380" s="1" t="s">
+        <v>1218</v>
+      </c>
+    </row>
+    <row r="1381" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1381" s="1" t="s">
+        <v>1219</v>
+      </c>
+    </row>
+    <row r="1382" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1382" s="1" t="s">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="1383" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1383" s="1" t="s">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="1384" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1384" s="1" t="s">
+        <v>1222</v>
+      </c>
+    </row>
+    <row r="1385" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1385" s="1" t="s">
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="1386" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1386" s="1" t="s">
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="1387" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1387" s="1" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="1388" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1388" s="1" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="1389" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1389" s="1" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="1390" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1390" s="1" t="s">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="1391" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1391" s="1" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="1392" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1392" s="1" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="1393" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1393" s="1" t="s">
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="1394" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1394" s="1" t="s">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="1395" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1395" s="1" t="s">
+        <v>1233</v>
+      </c>
+    </row>
+    <row r="1396" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1396" s="1" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="1397" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1397" s="1" t="s">
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="1398" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1398" s="1" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="1399" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1399" s="1" t="s">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="1400" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1400" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="1401" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1401" s="1" t="s">
+        <v>1238</v>
+      </c>
+    </row>
+    <row r="1402" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1402" s="1" t="s">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="1403" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1403" s="1" t="s">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="1404" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1404" s="1" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="1405" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1405" s="1" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="1406" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1406" s="1" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="1407" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1407" s="1" t="s">
+        <v>1244</v>
+      </c>
+    </row>
+    <row r="1408" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1408" s="1" t="s">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="1409" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1409" s="1" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="1410" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1410" s="1" t="s">
+        <v>1247</v>
+      </c>
+    </row>
+    <row r="1411" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1411" s="1" t="s">
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="1412" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1412" s="1" t="s">
+        <v>1249</v>
+      </c>
+    </row>
+    <row r="1413" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1413" s="1" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="1414" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1414" s="1" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="1415" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1415" s="1" t="s">
+        <v>1252</v>
+      </c>
+    </row>
+    <row r="1416" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1416" s="1" t="s">
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="1417" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1417" s="1" t="s">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="1418" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1418" s="1" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="1419" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1419" s="1" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="1420" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1420" s="1" t="s">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="1421" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1421" s="1" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="1422" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1422" s="1" t="s">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="1423" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1423" s="1" t="s">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="1424" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1424" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="1425" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1425" s="1" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="1426" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1426" s="1" t="s">
+        <v>1262</v>
+      </c>
+    </row>
+    <row r="1427" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1427" s="1" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="1428" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1428" s="1" t="s">
+        <v>1264</v>
+      </c>
+    </row>
+    <row r="1429" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1429" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1430" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1430" s="1" t="s">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="1431" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1431" s="1" t="s">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="1432" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1432" s="1" t="s">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="1433" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1433" s="1" t="s">
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="1434" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1434" s="1" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="1435" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1435" s="1" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="1436" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1436" s="1" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="1437" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1437" s="1" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="1438" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1438" s="1" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="1439" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1439" s="1" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="1440" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1440" s="1" t="s">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="1441" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1441" s="1" t="s">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="1442" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1442" s="1" t="s">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="1443" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1443" s="1" t="s">
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="1444" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1444" s="1" t="s">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="1445" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1445" s="1" t="s">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="1446" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1446" s="1" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="1447" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1447" s="1" t="s">
+        <v>1278</v>
+      </c>
+    </row>
+    <row r="1448" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1448" s="1" t="s">
+        <v>1279</v>
+      </c>
+    </row>
+    <row r="1449" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1449" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="1450" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1450" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1451" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1451" s="1" t="s">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="1452" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1452" s="1" t="s">
+        <v>1281</v>
+      </c>
+    </row>
+    <row r="1453" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1453" s="1" t="s">
+        <v>1282</v>
+      </c>
+    </row>
+    <row r="1454" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1454" s="1" t="s">
+        <v>1283</v>
+      </c>
+    </row>
+    <row r="1455" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1455" s="1" t="s">
+        <v>1284</v>
+      </c>
+    </row>
+    <row r="1456" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1456" s="1" t="s">
+        <v>1285</v>
+      </c>
+    </row>
+    <row r="1457" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1457" s="1" t="s">
+        <v>1286</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>